<commit_message>
Alinear generadores de PDF con diseño aprobado (commit 85bd06d) y agregar soporte completo de base de datos
- Actualizar pdfLabelGenerator.js con diseño aprobado por cliente:
  * Ajustar tamaños de fuente (título 8pt, fecha 6pt, serial 8pt)
  * Reposicionar elementos (QR en 18,11; logo en 4,23; serial en 35)
  * Agregar dos puntos y acentos a etiquetas (ENCARGADO:, UBICACIÓN:)

- Actualizar batchPdfGenerator.js con mismo diseño para consistencia

- Agregar migraciones de base de datos:
  * create_auxiliary_tables.sql: crear tablas locations, responsibles, asset_names
  * 003_add_name_field.sql: agregar columna name a tabla assets

- Actualizar rutas y plantillas para soporte completo del sistema
</commit_message>
<xml_diff>
--- a/public/templates/plantilla_activos.xlsx
+++ b/public/templates/plantilla_activos.xlsx
@@ -402,13 +402,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="50.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -416,22 +416,22 @@
         <v>Nombre</v>
       </c>
       <c r="B1" t="str">
-        <v>Descripción</v>
+        <v>Categoría</v>
       </c>
       <c r="C1" t="str">
+        <v>Estado</v>
+      </c>
+      <c r="D1" t="str">
         <v>Responsable</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Ubicación</v>
       </c>
-      <c r="E1" t="str">
-        <v>Categoría</v>
-      </c>
       <c r="F1" t="str">
+        <v>Observación o nota</v>
+      </c>
+      <c r="G1" t="str">
         <v>Valor</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Estado</v>
       </c>
     </row>
     <row r="2">
@@ -439,22 +439,22 @@
         <v>Laptop Dell Latitude 5420</v>
       </c>
       <c r="B2" t="str">
-        <v>Laptop corporativa Intel i7 16GB RAM</v>
+        <v>Equipo de Cómputo</v>
       </c>
       <c r="C2" t="str">
+        <v>Activo</v>
+      </c>
+      <c r="D2" t="str">
         <v>Juan Pérez</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>Oficina Principal</v>
       </c>
-      <c r="E2" t="str">
-        <v>Equipo de Cómputo</v>
-      </c>
       <c r="F2" t="str">
+        <v>Intel i7 16GB RAM, pantalla 14 pulgadas</v>
+      </c>
+      <c r="G2" t="str">
         <v>25000</v>
-      </c>
-      <c r="G2" t="str">
-        <v>Activo</v>
       </c>
     </row>
     <row r="3">
@@ -462,22 +462,22 @@
         <v>Monitor LG 27"</v>
       </c>
       <c r="B3" t="str">
-        <v>Monitor LED Full HD</v>
+        <v>Monitores</v>
       </c>
       <c r="C3" t="str">
+        <v>Activo</v>
+      </c>
+      <c r="D3" t="str">
         <v>María García</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <v>Sala de Juntas</v>
       </c>
-      <c r="E3" t="str">
-        <v>Monitores</v>
-      </c>
       <c r="F3" t="str">
+        <v>Monitor LED Full HD 1920x1080</v>
+      </c>
+      <c r="G3" t="str">
         <v>5500</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Activo</v>
       </c>
     </row>
     <row r="4">
@@ -485,22 +485,22 @@
         <v>Teclado Logitech MX Keys</v>
       </c>
       <c r="B4" t="str">
-        <v>Teclado inalámbrico mecánico</v>
+        <v>Periféricos</v>
       </c>
       <c r="C4" t="str">
+        <v>Activo</v>
+      </c>
+      <c r="D4" t="str">
         <v>Carlos López</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4" t="str">
         <v>Área de Desarrollo</v>
       </c>
-      <c r="E4" t="str">
-        <v>Periféricos</v>
-      </c>
       <c r="F4" t="str">
+        <v>Teclado inalámbrico mecánico retroiluminado</v>
+      </c>
+      <c r="G4" t="str">
         <v>2500</v>
-      </c>
-      <c r="G4" t="str">
-        <v>Activo</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: mejorar plantillas Excel con formato tabla y corregir descarga
- Instalar exceljs para generar plantillas con formato de tabla profesional
- Reorganizar rutas bulk en locations.js y responsibles.js (antes de /:id)
- Corregir funciones de descarga usando enlace temporal en lugar de window.open
- Regenerar plantillas con ExcelJS: colores, filtros y hoja de instrucciones
- Agregar script generateTemplatesExcelJS.js para regenerar plantillas
</commit_message>
<xml_diff>
--- a/public/templates/plantilla_activos.xlsx
+++ b/public/templates/plantilla_activos.xlsx
@@ -1,55 +1,173 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Activos" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Activos" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Instrucciones" state="visible" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Ubicación</t>
+  </si>
+  <si>
+    <t>Observación o nota</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Laptop Dell Latitude 5420</t>
+  </si>
+  <si>
+    <t>Equipos de Cómputo</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Juan Pérez</t>
+  </si>
+  <si>
+    <t>Oficina Principal</t>
+  </si>
+  <si>
+    <t>Equipo nuevo asignado</t>
+  </si>
+  <si>
+    <t>Monitor LG 24"</t>
+  </si>
+  <si>
+    <t>Periféricos</t>
+  </si>
+  <si>
+    <t>María García</t>
+  </si>
+  <si>
+    <t>Sala de Reuniones</t>
+  </si>
+  <si>
+    <t>Monitor secundario</t>
+  </si>
+  <si>
+    <t>Silla Ergonómica</t>
+  </si>
+  <si>
+    <t>Mobiliario</t>
+  </si>
+  <si>
+    <t>Carlos López</t>
+  </si>
+  <si>
+    <t>Área de Desarrollo</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>INSTRUCCIONES PARA CARGA MASIVA DE ACTIVOS</t>
+  </si>
+  <si>
+    <t>1. Complete la información en la hoja "Activos"</t>
+  </si>
+  <si>
+    <t>2. Puede eliminar las filas de ejemplo antes de agregar sus datos</t>
+  </si>
+  <si>
+    <t>3. El número de serie se genera AUTOMÁTICAMENTE, no lo incluya</t>
+  </si>
+  <si>
+    <t>CAMPOS:</t>
+  </si>
+  <si>
+    <t>• Nombre (Requerido): Nombre descriptivo del activo</t>
+  </si>
+  <si>
+    <t>• Categoría (Opcional): Tipo o categoría del activo</t>
+  </si>
+  <si>
+    <t>• Estado (Opcional): Estado del activo (por defecto: "Activo")</t>
+  </si>
+  <si>
+    <t>• Responsable (Requerido): Persona encargada del activo</t>
+  </si>
+  <si>
+    <t>• Ubicación (Requerido): Lugar donde se encuentra el activo</t>
+  </si>
+  <si>
+    <t>• Observación o nota (Opcional): Comentarios adicionales</t>
+  </si>
+  <si>
+    <t>• Valor (Opcional): Valor monetario del activo</t>
+  </si>
+  <si>
+    <t>NOTAS IMPORTANTES:</t>
+  </si>
+  <si>
+    <t>• Asegúrese de que los responsables y ubicaciones existan en el sistema</t>
+  </si>
+  <si>
+    <t>• El sistema generará automáticamente el código QR para cada activo</t>
+  </si>
+  <si>
+    <t>• Guarde el archivo en formato .xlsx antes de subirlo</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFF"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="4472C4"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="4472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,15 +182,52 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="TablaActivos" displayName="TablaActivos" ref="A1:G4" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:G4">
+    <filterColumn colId="0" hiddenButton="0"/>
+    <filterColumn colId="1" hiddenButton="0"/>
+    <filterColumn colId="2" hiddenButton="0"/>
+    <filterColumn colId="3" hiddenButton="0"/>
+    <filterColumn colId="4" hiddenButton="0"/>
+    <filterColumn colId="5" hiddenButton="0"/>
+    <filterColumn colId="6" hiddenButton="0"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Nombre" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Categoría" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Estado" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Responsable" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Ubicación" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Observación o nota" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Valor" totalsRowFunction="none"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,116 +551,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="4472C4"/>
+  </sheetPr>
   <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" customWidth="1"/>
-    <col min="6" max="6" width="50.83203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="40" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Nombre</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Categoría</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Estado</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Responsable</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Ubicación</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Observación o nota</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Valor</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Laptop Dell Latitude 5420</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Equipo de Cómputo</v>
-      </c>
-      <c r="C2" t="str">
-        <v>Activo</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Juan Pérez</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Oficina Principal</v>
-      </c>
-      <c r="F2" t="str">
-        <v>Intel i7 16GB RAM, pantalla 14 pulgadas</v>
-      </c>
-      <c r="G2" t="str">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Monitor LG 27"</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Monitores</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Activo</v>
-      </c>
-      <c r="D3" t="str">
-        <v>María García</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Sala de Juntas</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Monitor LED Full HD 1920x1080</v>
-      </c>
-      <c r="G3" t="str">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Teclado Logitech MX Keys</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Periféricos</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Activo</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Carlos López</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Área de Desarrollo</v>
-      </c>
-      <c r="F4" t="str">
-        <v>Teclado inalámbrico mecánico retroiluminado</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2500</v>
+    <row r="1" ht="25" customHeight="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="70AD47"/>
+  </sheetPr>
+  <dimension ref="A1:A19"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="80" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>